<commit_message>
Signed-off-by: Tharindu Rajindra Piyasekara <t.rajindra@gmail.com>
</commit_message>
<xml_diff>
--- a/Daily Progress Report.xlsx
+++ b/Daily Progress Report.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>High</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>Indentify limitation of the device</t>
+  </si>
+  <si>
+    <t>Normal</t>
   </si>
 </sst>
 </file>
@@ -288,20 +291,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1" tint="0.24994659260841701"/>
-        <name val="Franklin Gothic Medium"/>
-        <scheme val="major"/>
-      </font>
-      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color theme="1" tint="0.24994659260841701"/>
         <name val="Bookman Old Style"/>
@@ -315,6 +304,20 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <name val="Franklin Gothic Medium"/>
+        <scheme val="major"/>
+      </font>
+      <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -501,16 +504,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ToDoList" displayName="ToDoList" ref="C5:J14" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ToDoList" displayName="ToDoList" ref="C5:J14" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="C5:J14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="TASK"/>
     <tableColumn id="3" name="PRIORITY "/>
     <tableColumn id="4" name="STATUS "/>
-    <tableColumn id="6" name="START DATE " dataDxfId="5"/>
-    <tableColumn id="7" name="DUE DATE " dataDxfId="4"/>
+    <tableColumn id="6" name="START DATE " dataDxfId="4"/>
+    <tableColumn id="7" name="DUE DATE " dataDxfId="3"/>
     <tableColumn id="5" name="% COMPLETE" dataCellStyle="Percent"/>
-    <tableColumn id="9" name="DONE?" dataDxfId="3">
+    <tableColumn id="9" name="DONE?" dataDxfId="2">
       <calculatedColumnFormula>--(ToDoList[[#This Row],[% COMPLETE]]=1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" name="NOTES"/>
@@ -753,7 +756,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="24" customHeight="1"/>
@@ -855,11 +858,19 @@
       <c r="C10" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="10"/>
+      <c r="D10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="14">
+        <v>41821</v>
+      </c>
       <c r="G10" s="10"/>
-      <c r="H10" s="3"/>
+      <c r="H10" s="3">
+        <v>0.25</v>
+      </c>
       <c r="I10" s="17"/>
       <c r="J10" s="2"/>
     </row>
@@ -867,14 +878,27 @@
       <c r="C11" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="15"/>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="14">
+        <v>41821</v>
+      </c>
       <c r="G11" s="15"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7">
+        <v>0.25</v>
+      </c>
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:10" ht="24" customHeight="1">
       <c r="C12" s="11" t="s">
         <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
       </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
@@ -884,6 +908,9 @@
     <row r="13" spans="1:10" ht="24" customHeight="1">
       <c r="C13" s="11" t="s">
         <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -897,6 +924,9 @@
       <c r="C14" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
       <c r="H14" s="7"/>
@@ -907,8 +937,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D10:J14 C9:J9">
-    <cfRule type="expression" dxfId="0" priority="4">
+  <conditionalFormatting sqref="C9:J9 D10:J14">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>$H9=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Project Proposal & sample Desktop project
</commit_message>
<xml_diff>
--- a/Daily Progress Report.xlsx
+++ b/Daily Progress Report.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
-    <sheet name="To-Do List" sheetId="1" r:id="rId1"/>
+    <sheet name="Daily Progress Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">ToDoList[#All]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'To-Do List'!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Daily Progress Report'!$3:$3</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -269,14 +269,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <fill>
         <patternFill>
@@ -318,13 +311,6 @@
         <scheme val="major"/>
       </font>
       <alignment vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <border>
@@ -471,20 +457,20 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="To-Do List" defaultPivotStyle="PivotStyleLight2">
     <tableStyle name="To Do List Pivot" table="0" count="11">
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="totalRow" dxfId="17"/>
-      <tableStyleElement type="firstRowStripe" dxfId="16"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="15"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="14"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="13"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="11"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="10"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="9"/>
-      <tableStyleElement type="pageFieldValues" dxfId="8"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="12"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="10"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="9"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="8"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="7"/>
+      <tableStyleElement type="pageFieldValues" dxfId="6"/>
     </tableStyle>
     <tableStyle name="To-Do List" pivot="0" count="1">
-      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -504,16 +490,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ToDoList" displayName="ToDoList" ref="C5:J14" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="ToDoList" displayName="ToDoList" ref="C5:J14" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="C5:J14"/>
   <tableColumns count="8">
     <tableColumn id="1" name="TASK"/>
     <tableColumn id="3" name="PRIORITY "/>
     <tableColumn id="4" name="STATUS "/>
-    <tableColumn id="6" name="START DATE " dataDxfId="4"/>
-    <tableColumn id="7" name="DUE DATE " dataDxfId="3"/>
+    <tableColumn id="6" name="START DATE " dataDxfId="3"/>
+    <tableColumn id="7" name="DUE DATE " dataDxfId="2"/>
     <tableColumn id="5" name="% COMPLETE" dataCellStyle="Percent"/>
-    <tableColumn id="9" name="DONE?" dataDxfId="2">
+    <tableColumn id="9" name="DONE?" dataDxfId="1">
       <calculatedColumnFormula>--(ToDoList[[#This Row],[% COMPLETE]]=1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="10" name="NOTES"/>
@@ -756,7 +742,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="24" customHeight="1"/>
@@ -938,7 +924,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C9:J9 D10:J14">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$H9=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>